<commit_message>
done sending file i guess?
</commit_message>
<xml_diff>
--- a/SimpO - Copy.xlsx
+++ b/SimpO - Copy.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SimpO_HTTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E2614C-24F6-4721-AF99-3FE7C98DC89C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="26295" windowHeight="14175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -567,9 +566,6 @@
     <t>chuongngaivat</t>
   </si>
   <si>
-    <t>image.png</t>
-  </si>
-  <si>
     <t>vcnv 1</t>
   </si>
   <si>
@@ -615,27 +611,15 @@
     <t>đa tt 1</t>
   </si>
   <si>
-    <t>tt1.mp4</t>
-  </si>
-  <si>
     <t>đa tt 2</t>
   </si>
   <si>
-    <t>tt1.mp5</t>
-  </si>
-  <si>
     <t>đa tt 3</t>
   </si>
   <si>
-    <t>tt1.mp6</t>
-  </si>
-  <si>
     <t>đa tt 4</t>
   </si>
   <si>
-    <t>tt1.mp7</t>
-  </si>
-  <si>
     <t>vđ 1</t>
   </si>
   <si>
@@ -796,12 +780,27 @@
   </si>
   <si>
     <t>đa 36</t>
+  </si>
+  <si>
+    <t>ảnhcnv.png</t>
+  </si>
+  <si>
+    <t>tt1.png</t>
+  </si>
+  <si>
+    <t>tt2.png</t>
+  </si>
+  <si>
+    <t>tt3.png</t>
+  </si>
+  <si>
+    <t>tt4.mp4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1454,6 +1453,24 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1463,15 +1480,36 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1499,21 +1537,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1524,30 +1547,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1835,146 +1834,146 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H103" sqref="H103"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="48.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="4.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="48.875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
-    <col min="12" max="12" width="48.88671875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="48.875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1" customWidth="1"/>
     <col min="16" max="16" width="10" style="1" customWidth="1"/>
-    <col min="17" max="17" width="48.88671875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="26.44140625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="12.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="48.875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="26.5" style="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
+      <c r="A2" s="66"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
+      <c r="A3" s="66"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
+      <c r="A4" s="66"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-    </row>
-    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+    </row>
+    <row r="6" spans="1:9" ht="17.100000000000001" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="63"/>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
-      <c r="H7" s="63"/>
-      <c r="I7" s="64"/>
-    </row>
-    <row r="8" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="65"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="61"/>
+    </row>
+    <row r="8" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="62"/>
       <c r="B8" s="80"/>
       <c r="C8" s="80"/>
       <c r="D8" s="80"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
       <c r="G8" s="80"/>
       <c r="H8" s="80"/>
       <c r="I8" s="81"/>
     </row>
-    <row r="9" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="74"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="72" t="s">
+      <c r="G9" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H9" s="73"/>
-      <c r="I9" s="74"/>
-    </row>
-    <row r="10" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="49"/>
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="77"/>
+      <c r="B10" s="51"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="53"/>
       <c r="E10" s="3"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="75"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="77"/>
-    </row>
-    <row r="11" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="51"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
+    </row>
+    <row r="11" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="5" t="s">
         <v>5</v>
@@ -1997,7 +1996,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1</v>
       </c>
@@ -2020,7 +2019,7 @@
       </c>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2</v>
       </c>
@@ -2043,7 +2042,7 @@
       </c>
       <c r="I13" s="23"/>
     </row>
-    <row r="14" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -2066,7 +2065,7 @@
       </c>
       <c r="I14" s="23"/>
     </row>
-    <row r="15" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -2089,7 +2088,7 @@
       </c>
       <c r="I15" s="23"/>
     </row>
-    <row r="16" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>5</v>
       </c>
@@ -2112,7 +2111,7 @@
       </c>
       <c r="I16" s="23"/>
     </row>
-    <row r="17" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>6</v>
       </c>
@@ -2135,7 +2134,7 @@
       </c>
       <c r="I17" s="23"/>
     </row>
-    <row r="18" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>7</v>
       </c>
@@ -2158,7 +2157,7 @@
       </c>
       <c r="I18" s="23"/>
     </row>
-    <row r="19" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>8</v>
       </c>
@@ -2181,7 +2180,7 @@
       </c>
       <c r="I19" s="23"/>
     </row>
-    <row r="20" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>9</v>
       </c>
@@ -2204,7 +2203,7 @@
       </c>
       <c r="I20" s="23"/>
     </row>
-    <row r="21" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>10</v>
       </c>
@@ -2227,7 +2226,7 @@
       </c>
       <c r="I21" s="23"/>
     </row>
-    <row r="22" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>11</v>
       </c>
@@ -2250,7 +2249,7 @@
       </c>
       <c r="I22" s="23"/>
     </row>
-    <row r="23" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>12</v>
       </c>
@@ -2273,7 +2272,7 @@
       </c>
       <c r="I23" s="23"/>
     </row>
-    <row r="24" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>13</v>
       </c>
@@ -2296,7 +2295,7 @@
       </c>
       <c r="I24" s="23"/>
     </row>
-    <row r="25" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>14</v>
       </c>
@@ -2319,7 +2318,7 @@
       </c>
       <c r="I25" s="23"/>
     </row>
-    <row r="26" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>15</v>
       </c>
@@ -2342,7 +2341,7 @@
       </c>
       <c r="I26" s="23"/>
     </row>
-    <row r="27" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>16</v>
       </c>
@@ -2365,7 +2364,7 @@
       </c>
       <c r="I27" s="23"/>
     </row>
-    <row r="28" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>17</v>
       </c>
@@ -2388,7 +2387,7 @@
       </c>
       <c r="I28" s="23"/>
     </row>
-    <row r="29" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>18</v>
       </c>
@@ -2411,7 +2410,7 @@
       </c>
       <c r="I29" s="23"/>
     </row>
-    <row r="30" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>19</v>
       </c>
@@ -2434,7 +2433,7 @@
       </c>
       <c r="I30" s="23"/>
     </row>
-    <row r="31" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>20</v>
       </c>
@@ -2457,7 +2456,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2468,33 +2467,33 @@
       <c r="H32" s="8"/>
       <c r="I32" s="11"/>
     </row>
-    <row r="33" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="73"/>
-      <c r="D33" s="74"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="50"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
-      <c r="G33" s="72" t="s">
+      <c r="G33" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="73"/>
-      <c r="I33" s="74"/>
-    </row>
-    <row r="34" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H33" s="49"/>
+      <c r="I33" s="50"/>
+    </row>
+    <row r="34" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
-      <c r="B34" s="75"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="77"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="53"/>
       <c r="E34" s="3"/>
       <c r="F34" s="8"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="77"/>
-    </row>
-    <row r="35" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="51"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="53"/>
+    </row>
+    <row r="35" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="5" t="s">
         <v>5</v>
@@ -2517,7 +2516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -2540,7 +2539,7 @@
       </c>
       <c r="I36" s="22"/>
     </row>
-    <row r="37" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -2563,7 +2562,7 @@
       </c>
       <c r="I37" s="23"/>
     </row>
-    <row r="38" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -2586,7 +2585,7 @@
       </c>
       <c r="I38" s="23"/>
     </row>
-    <row r="39" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -2609,7 +2608,7 @@
       </c>
       <c r="I39" s="23"/>
     </row>
-    <row r="40" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>5</v>
       </c>
@@ -2632,7 +2631,7 @@
       </c>
       <c r="I40" s="23"/>
     </row>
-    <row r="41" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>6</v>
       </c>
@@ -2655,7 +2654,7 @@
       </c>
       <c r="I41" s="23"/>
     </row>
-    <row r="42" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>7</v>
       </c>
@@ -2678,7 +2677,7 @@
       </c>
       <c r="I42" s="23"/>
     </row>
-    <row r="43" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>8</v>
       </c>
@@ -2701,7 +2700,7 @@
       </c>
       <c r="I43" s="23"/>
     </row>
-    <row r="44" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -2724,7 +2723,7 @@
       </c>
       <c r="I44" s="23"/>
     </row>
-    <row r="45" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -2747,7 +2746,7 @@
       </c>
       <c r="I45" s="23"/>
     </row>
-    <row r="46" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>11</v>
       </c>
@@ -2770,7 +2769,7 @@
       </c>
       <c r="I46" s="23"/>
     </row>
-    <row r="47" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -2793,7 +2792,7 @@
       </c>
       <c r="I47" s="23"/>
     </row>
-    <row r="48" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>13</v>
       </c>
@@ -2816,7 +2815,7 @@
       </c>
       <c r="I48" s="23"/>
     </row>
-    <row r="49" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>14</v>
       </c>
@@ -2839,7 +2838,7 @@
       </c>
       <c r="I49" s="23"/>
     </row>
-    <row r="50" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -2862,7 +2861,7 @@
       </c>
       <c r="I50" s="23"/>
     </row>
-    <row r="51" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -2885,7 +2884,7 @@
       </c>
       <c r="I51" s="23"/>
     </row>
-    <row r="52" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>17</v>
       </c>
@@ -2912,7 +2911,7 @@
       <c r="M52" s="35"/>
       <c r="N52" s="35"/>
     </row>
-    <row r="53" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>18</v>
       </c>
@@ -2939,7 +2938,7 @@
       <c r="M53" s="35"/>
       <c r="N53" s="35"/>
     </row>
-    <row r="54" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>19</v>
       </c>
@@ -2966,7 +2965,7 @@
       <c r="M54" s="35"/>
       <c r="N54" s="35"/>
     </row>
-    <row r="55" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>20</v>
       </c>
@@ -2993,7 +2992,7 @@
       <c r="M55" s="35"/>
       <c r="N55" s="35"/>
     </row>
-    <row r="56" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="8"/>
       <c r="B56" s="36"/>
       <c r="C56" s="36"/>
@@ -3008,7 +3007,7 @@
       <c r="M56" s="35"/>
       <c r="N56" s="35"/>
     </row>
-    <row r="57" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="8"/>
       <c r="C57" s="8"/>
@@ -3019,39 +3018,39 @@
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
     </row>
-    <row r="58" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="53" t="s">
+    <row r="58" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B58" s="54"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="55"/>
-      <c r="F58" s="53" t="s">
+      <c r="B58" s="67"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="68"/>
+      <c r="F58" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="G58" s="63"/>
-      <c r="H58" s="63"/>
-      <c r="I58" s="64"/>
-    </row>
-    <row r="59" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="56"/>
-      <c r="B59" s="57"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="58"/>
-      <c r="F59" s="65"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="66"/>
-      <c r="I59" s="67"/>
-    </row>
-    <row r="60" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="68" t="s">
+      <c r="G58" s="60"/>
+      <c r="H58" s="60"/>
+      <c r="I58" s="61"/>
+    </row>
+    <row r="59" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="69"/>
+      <c r="B59" s="70"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="71"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="64"/>
+    </row>
+    <row r="60" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="76" t="s">
         <v>17</v>
       </c>
-      <c r="B60" s="69"/>
-      <c r="C60" s="70" t="s">
+      <c r="B60" s="77"/>
+      <c r="C60" s="78" t="s">
         <v>179</v>
       </c>
-      <c r="D60" s="71"/>
+      <c r="D60" s="79"/>
       <c r="F60" s="37" t="s">
         <v>8</v>
       </c>
@@ -3065,29 +3064,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="59" t="s">
+    <row r="61" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B61" s="60"/>
-      <c r="C61" s="61" t="s">
-        <v>180</v>
-      </c>
-      <c r="D61" s="62"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="74" t="s">
+        <v>252</v>
+      </c>
+      <c r="D61" s="75"/>
       <c r="F61" s="38">
         <v>1</v>
       </c>
       <c r="G61" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H61" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I61" s="22" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="44" t="s">
         <v>15</v>
       </c>
@@ -3104,159 +3103,159 @@
         <v>2</v>
       </c>
       <c r="G62" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H62" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="38">
         <v>1</v>
       </c>
       <c r="B63" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C63" s="29" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D63" s="25"/>
       <c r="F63" s="39">
         <v>3</v>
       </c>
       <c r="G63" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H63" s="31" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="39">
         <v>2</v>
       </c>
       <c r="B64" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C64" s="29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D64" s="26"/>
       <c r="F64" s="40">
         <v>4</v>
       </c>
       <c r="G64" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H64" s="31" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I64" s="22" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="39">
         <v>3</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C65" s="29" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D65" s="26"/>
     </row>
-    <row r="66" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="39">
         <v>4</v>
       </c>
       <c r="B66" s="28" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C66" s="29" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D66" s="26"/>
     </row>
-    <row r="67" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B67" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C67" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="C67" s="29" t="s">
-        <v>190</v>
-      </c>
       <c r="D67" s="27"/>
     </row>
-    <row r="68" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="46"/>
       <c r="B68" s="47"/>
       <c r="C68" s="47"/>
       <c r="D68" s="47"/>
     </row>
-    <row r="69" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="53" t="s">
+    <row r="69" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B72" s="63"/>
-      <c r="C72" s="63"/>
-      <c r="D72" s="63"/>
-      <c r="E72" s="63"/>
-      <c r="F72" s="63"/>
-      <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="64"/>
-    </row>
-    <row r="73" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="65"/>
-      <c r="B73" s="66"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
-      <c r="H73" s="66"/>
-      <c r="I73" s="67"/>
-    </row>
-    <row r="74" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="60"/>
+      <c r="C72" s="60"/>
+      <c r="D72" s="60"/>
+      <c r="E72" s="60"/>
+      <c r="F72" s="60"/>
+      <c r="G72" s="60"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="61"/>
+    </row>
+    <row r="73" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="62"/>
+      <c r="B73" s="63"/>
+      <c r="C73" s="63"/>
+      <c r="D73" s="63"/>
+      <c r="E73" s="63"/>
+      <c r="F73" s="63"/>
+      <c r="G73" s="63"/>
+      <c r="H73" s="63"/>
+      <c r="I73" s="64"/>
+    </row>
+    <row r="74" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
-      <c r="B74" s="72" t="s">
+      <c r="B74" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C74" s="73"/>
-      <c r="D74" s="74"/>
+      <c r="C74" s="49"/>
+      <c r="D74" s="50"/>
       <c r="E74" s="3"/>
       <c r="F74" s="4"/>
-      <c r="G74" s="72" t="s">
+      <c r="G74" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H74" s="73"/>
-      <c r="I74" s="74"/>
-    </row>
-    <row r="75" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H74" s="49"/>
+      <c r="I74" s="50"/>
+    </row>
+    <row r="75" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
-      <c r="B75" s="75"/>
-      <c r="C75" s="76"/>
-      <c r="D75" s="77"/>
+      <c r="B75" s="51"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="53"/>
       <c r="E75" s="8"/>
       <c r="F75" s="8"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="76"/>
-      <c r="I75" s="77"/>
-    </row>
-    <row r="76" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G75" s="51"/>
+      <c r="H75" s="52"/>
+      <c r="I75" s="53"/>
+    </row>
+    <row r="76" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="5" t="s">
         <v>5</v>
@@ -3279,190 +3278,190 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="79" t="s">
+    <row r="77" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D77" s="34"/>
       <c r="E77" s="11"/>
-      <c r="F77" s="79" t="s">
+      <c r="F77" s="58" t="s">
         <v>10</v>
       </c>
       <c r="G77" s="32" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="H77" s="33" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="I77" s="34"/>
     </row>
-    <row r="78" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="49"/>
+    <row r="78" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="55"/>
       <c r="B78" s="32" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D78" s="23"/>
       <c r="E78" s="11"/>
-      <c r="F78" s="49"/>
+      <c r="F78" s="55"/>
       <c r="G78" s="32" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H78" s="33" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="I78" s="23"/>
     </row>
-    <row r="79" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="78"/>
+    <row r="79" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="57"/>
       <c r="B79" s="32" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D79" s="24"/>
       <c r="E79" s="11"/>
-      <c r="F79" s="78"/>
+      <c r="F79" s="57"/>
       <c r="G79" s="32" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="H79" s="33" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="I79" s="24"/>
     </row>
-    <row r="80" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="48" t="s">
+    <row r="80" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="54" t="s">
         <v>11</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="D80" s="34"/>
       <c r="E80" s="11"/>
-      <c r="F80" s="48" t="s">
+      <c r="F80" s="54" t="s">
         <v>11</v>
       </c>
       <c r="G80" s="32" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H80" s="33" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="I80" s="34"/>
     </row>
-    <row r="81" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="49"/>
+    <row r="81" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="55"/>
       <c r="B81" s="32" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="11"/>
-      <c r="F81" s="49"/>
+      <c r="F81" s="55"/>
       <c r="G81" s="32" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="H81" s="33" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="I81" s="23"/>
     </row>
-    <row r="82" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="78"/>
+    <row r="82" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="57"/>
       <c r="B82" s="32" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D82" s="24"/>
       <c r="E82" s="11"/>
-      <c r="F82" s="78"/>
+      <c r="F82" s="57"/>
       <c r="G82" s="32" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H82" s="33" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I82" s="24"/>
     </row>
-    <row r="83" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="48" t="s">
+    <row r="83" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="54" t="s">
         <v>12</v>
       </c>
       <c r="B83" s="32" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D83" s="22"/>
       <c r="E83" s="11"/>
-      <c r="F83" s="48" t="s">
+      <c r="F83" s="54" t="s">
         <v>12</v>
       </c>
       <c r="G83" s="32" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="H83" s="33" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I83" s="34"/>
     </row>
-    <row r="84" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="49"/>
+    <row r="84" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="55"/>
       <c r="B84" s="32" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="C84" s="33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D84" s="23"/>
       <c r="E84" s="11"/>
-      <c r="F84" s="49"/>
+      <c r="F84" s="55"/>
       <c r="G84" s="32" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="H84" s="33" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I84" s="23"/>
     </row>
-    <row r="85" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="50"/>
+    <row r="85" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="56"/>
       <c r="B85" s="32" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D85" s="24"/>
       <c r="E85" s="11"/>
-      <c r="F85" s="50"/>
+      <c r="F85" s="56"/>
       <c r="G85" s="32" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="H85" s="33" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I85" s="24"/>
     </row>
-    <row r="86" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" s="8"/>
       <c r="C86" s="8"/>
@@ -3473,33 +3472,33 @@
       <c r="H86" s="8"/>
       <c r="I86" s="11"/>
     </row>
-    <row r="87" spans="1:9" ht="22.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="C87" s="73"/>
-      <c r="D87" s="74"/>
+      <c r="C87" s="49"/>
+      <c r="D87" s="50"/>
       <c r="E87" s="3"/>
       <c r="F87" s="8"/>
-      <c r="G87" s="72" t="s">
+      <c r="G87" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="H87" s="73"/>
-      <c r="I87" s="74"/>
-    </row>
-    <row r="88" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H87" s="49"/>
+      <c r="I87" s="50"/>
+    </row>
+    <row r="88" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
-      <c r="B88" s="75"/>
-      <c r="C88" s="76"/>
-      <c r="D88" s="77"/>
+      <c r="B88" s="51"/>
+      <c r="C88" s="52"/>
+      <c r="D88" s="53"/>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
-      <c r="G88" s="75"/>
-      <c r="H88" s="76"/>
-      <c r="I88" s="77"/>
-    </row>
-    <row r="89" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G88" s="51"/>
+      <c r="H88" s="52"/>
+      <c r="I88" s="53"/>
+    </row>
+    <row r="89" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="16" t="s">
         <v>5</v>
@@ -3522,204 +3521,191 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="79" t="s">
+    <row r="90" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B90" s="32">
         <v>19</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D90" s="34"/>
       <c r="E90" s="11"/>
-      <c r="F90" s="79" t="s">
+      <c r="F90" s="58" t="s">
         <v>10</v>
       </c>
       <c r="G90" s="32">
         <v>28</v>
       </c>
       <c r="H90" s="33" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="I90" s="34"/>
     </row>
-    <row r="91" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="49"/>
+    <row r="91" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="55"/>
       <c r="B91" s="32">
         <v>20</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D91" s="23"/>
       <c r="E91" s="11"/>
-      <c r="F91" s="49"/>
+      <c r="F91" s="55"/>
       <c r="G91" s="32">
         <v>29</v>
       </c>
       <c r="H91" s="33" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I91" s="23"/>
     </row>
-    <row r="92" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="78"/>
+    <row r="92" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="57"/>
       <c r="B92" s="32">
         <v>21</v>
       </c>
       <c r="C92" s="33" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D92" s="24"/>
       <c r="E92" s="11"/>
-      <c r="F92" s="78"/>
+      <c r="F92" s="57"/>
       <c r="G92" s="32">
         <v>30</v>
       </c>
       <c r="H92" s="33" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="I92" s="24"/>
     </row>
-    <row r="93" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="48" t="s">
+    <row r="93" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="54" t="s">
         <v>11</v>
       </c>
       <c r="B93" s="32">
         <v>22</v>
       </c>
       <c r="C93" s="33" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D93" s="34"/>
       <c r="E93" s="11"/>
-      <c r="F93" s="48" t="s">
+      <c r="F93" s="54" t="s">
         <v>11</v>
       </c>
       <c r="G93" s="32">
         <v>31</v>
       </c>
       <c r="H93" s="33" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I93" s="34"/>
     </row>
-    <row r="94" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="49"/>
+    <row r="94" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="55"/>
       <c r="B94" s="32">
         <v>23</v>
       </c>
       <c r="C94" s="33" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D94" s="23"/>
       <c r="E94" s="11"/>
-      <c r="F94" s="49"/>
+      <c r="F94" s="55"/>
       <c r="G94" s="32">
         <v>32</v>
       </c>
       <c r="H94" s="33" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="I94" s="23"/>
     </row>
-    <row r="95" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="78"/>
+    <row r="95" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="57"/>
       <c r="B95" s="32">
         <v>24</v>
       </c>
       <c r="C95" s="33" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D95" s="24"/>
       <c r="E95" s="11"/>
-      <c r="F95" s="78"/>
+      <c r="F95" s="57"/>
       <c r="G95" s="32">
         <v>33</v>
       </c>
       <c r="H95" s="33" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I95" s="24"/>
     </row>
-    <row r="96" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="48" t="s">
+    <row r="96" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="54" t="s">
         <v>12</v>
       </c>
       <c r="B96" s="32">
         <v>25</v>
       </c>
       <c r="C96" s="33" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D96" s="34"/>
       <c r="E96" s="11"/>
-      <c r="F96" s="48" t="s">
+      <c r="F96" s="54" t="s">
         <v>12</v>
       </c>
       <c r="G96" s="32">
         <v>34</v>
       </c>
       <c r="H96" s="33" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="I96" s="34"/>
     </row>
-    <row r="97" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="49"/>
+    <row r="97" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="55"/>
       <c r="B97" s="32">
         <v>26</v>
       </c>
       <c r="C97" s="33" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D97" s="23"/>
       <c r="E97" s="11"/>
-      <c r="F97" s="49"/>
+      <c r="F97" s="55"/>
       <c r="G97" s="32">
         <v>35</v>
       </c>
       <c r="H97" s="33" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I97" s="23"/>
     </row>
-    <row r="98" spans="1:9" ht="22.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="50"/>
+    <row r="98" spans="1:9" ht="22.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="56"/>
       <c r="B98" s="32">
         <v>27</v>
       </c>
       <c r="C98" s="33" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D98" s="24"/>
       <c r="E98" s="19"/>
-      <c r="F98" s="50"/>
+      <c r="F98" s="56"/>
       <c r="G98" s="32">
         <v>36</v>
       </c>
       <c r="H98" s="33" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="I98" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G74:I75"/>
-    <mergeCell ref="G87:I88"/>
-    <mergeCell ref="F96:F98"/>
-    <mergeCell ref="F93:F95"/>
-    <mergeCell ref="F90:F92"/>
-    <mergeCell ref="F83:F85"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="F77:F79"/>
-    <mergeCell ref="F58:I59"/>
-    <mergeCell ref="G33:I34"/>
-    <mergeCell ref="B33:D34"/>
-    <mergeCell ref="G9:I10"/>
-    <mergeCell ref="B9:D10"/>
     <mergeCell ref="A96:A98"/>
     <mergeCell ref="A1:I5"/>
     <mergeCell ref="A58:D59"/>
@@ -3736,6 +3722,19 @@
     <mergeCell ref="A80:A82"/>
     <mergeCell ref="A77:A79"/>
     <mergeCell ref="A7:I8"/>
+    <mergeCell ref="F58:I59"/>
+    <mergeCell ref="G33:I34"/>
+    <mergeCell ref="B33:D34"/>
+    <mergeCell ref="G9:I10"/>
+    <mergeCell ref="B9:D10"/>
+    <mergeCell ref="G74:I75"/>
+    <mergeCell ref="G87:I88"/>
+    <mergeCell ref="F96:F98"/>
+    <mergeCell ref="F93:F95"/>
+    <mergeCell ref="F90:F92"/>
+    <mergeCell ref="F83:F85"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="F77:F79"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>